<commit_message>
Added post-processed files for 80/20 clr cross validation
- Added 'hole_id' index to initial train/test files so cross validation can be performed.
</commit_message>
<xml_diff>
--- a/_RESULTS/CROSS_VALIDATION_PREPROCESSED_CLR/Berg/GZ/GZ_1_train_pca.xlsx
+++ b/_RESULTS/CROSS_VALIDATION_PREPROCESSED_CLR/Berg/GZ/GZ_1_train_pca.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="42">
   <si>
     <t>lat</t>
   </si>
@@ -51,6 +51,93 @@
   </si>
   <si>
     <t>PC10</t>
+  </si>
+  <si>
+    <t>hole_id</t>
+  </si>
+  <si>
+    <t>BRG_16_07</t>
+  </si>
+  <si>
+    <t>BRG_16_03</t>
+  </si>
+  <si>
+    <t>BRG_16_04B</t>
+  </si>
+  <si>
+    <t>ECO_09_02</t>
+  </si>
+  <si>
+    <t>BRG_16_01</t>
+  </si>
+  <si>
+    <t>BRG_16_02</t>
+  </si>
+  <si>
+    <t>BRG_01_05</t>
+  </si>
+  <si>
+    <t>BRG_01_03</t>
+  </si>
+  <si>
+    <t>BRG_05_09</t>
+  </si>
+  <si>
+    <t>BRG_05_02</t>
+  </si>
+  <si>
+    <t>ECO_09_01</t>
+  </si>
+  <si>
+    <t>BRG_13_01</t>
+  </si>
+  <si>
+    <t>BRG_16_09</t>
+  </si>
+  <si>
+    <t>BRG_05_15</t>
+  </si>
+  <si>
+    <t>BRG_05_13</t>
+  </si>
+  <si>
+    <t>BRG_01_07</t>
+  </si>
+  <si>
+    <t>BRG_05_05</t>
+  </si>
+  <si>
+    <t>BRG_01_08</t>
+  </si>
+  <si>
+    <t>ECO_09_05</t>
+  </si>
+  <si>
+    <t>BRG_01_02</t>
+  </si>
+  <si>
+    <t>BRG_05_11</t>
+  </si>
+  <si>
+    <t>BRG_01_01</t>
+  </si>
+  <si>
+    <t>BRG_05_10</t>
+  </si>
+  <si>
+    <t>BRG_01_06</t>
+  </si>
+  <si>
+    <t>BRG_05_03</t>
+  </si>
+  <si>
+    <t>BRG_05_01</t>
+  </si>
+  <si>
+    <t>BRG_01_09</t>
+  </si>
+  <si>
+    <t>BRG_05_04</t>
   </si>
   <si>
     <t>train</t>
@@ -418,6 +505,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -456,8 +546,8 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2" s="1">
-        <v>0</v>
+      <c r="A2" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="B2">
         <v>50.96950109</v>
@@ -497,8 +587,8 @@
       </c>
     </row>
     <row r="3" spans="1:13">
-      <c r="A3" s="1">
-        <v>1</v>
+      <c r="A3" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="B3">
         <v>50.96729391</v>
@@ -538,8 +628,8 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="A4" s="1">
-        <v>2</v>
+      <c r="A4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B4">
         <v>50.96559512</v>
@@ -579,8 +669,8 @@
       </c>
     </row>
     <row r="5" spans="1:13">
-      <c r="A5" s="1">
-        <v>3</v>
+      <c r="A5" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B5">
         <v>50.96140111</v>
@@ -620,8 +710,8 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="1">
-        <v>4</v>
+      <c r="A6" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B6">
         <v>50.96504984</v>
@@ -661,8 +751,8 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="1">
-        <v>5</v>
+      <c r="A7" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B7">
         <v>50.96572401</v>
@@ -702,8 +792,8 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="1">
-        <v>6</v>
+      <c r="A8" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="B8">
         <v>50.96574917</v>
@@ -743,8 +833,8 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="1">
-        <v>7</v>
+      <c r="A9" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="B9">
         <v>50.96716463</v>
@@ -784,8 +874,8 @@
       </c>
     </row>
     <row r="10" spans="1:13">
-      <c r="A10" s="1">
-        <v>8</v>
+      <c r="A10" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="B10">
         <v>50.96812007</v>
@@ -825,8 +915,8 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="1">
-        <v>9</v>
+      <c r="A11" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B11">
         <v>50.96440023</v>
@@ -866,8 +956,8 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="1">
-        <v>10</v>
+      <c r="A12" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="B12">
         <v>50.95970242</v>
@@ -907,8 +997,8 @@
       </c>
     </row>
     <row r="13" spans="1:13">
-      <c r="A13" s="1">
-        <v>11</v>
+      <c r="A13" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B13">
         <v>50.96743469</v>
@@ -948,8 +1038,8 @@
       </c>
     </row>
     <row r="14" spans="1:13">
-      <c r="A14" s="1">
-        <v>12</v>
+      <c r="A14" s="1" t="s">
+        <v>25</v>
       </c>
       <c r="B14">
         <v>50.96757544</v>
@@ -989,8 +1079,8 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="1">
-        <v>13</v>
+      <c r="A15" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B15">
         <v>50.96384614</v>
@@ -1030,8 +1120,8 @@
       </c>
     </row>
     <row r="16" spans="1:13">
-      <c r="A16" s="1">
-        <v>14</v>
+      <c r="A16" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="B16">
         <v>50.96661119</v>
@@ -1071,8 +1161,8 @@
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="1">
-        <v>15</v>
+      <c r="A17" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="B17">
         <v>50.96544421</v>
@@ -1112,8 +1202,8 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="1">
-        <v>16</v>
+      <c r="A18" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B18">
         <v>50.9678689</v>
@@ -1153,8 +1243,8 @@
       </c>
     </row>
     <row r="19" spans="1:13">
-      <c r="A19" s="1">
-        <v>17</v>
+      <c r="A19" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B19">
         <v>50.96586666</v>
@@ -1194,8 +1284,8 @@
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="1">
-        <v>18</v>
+      <c r="A20" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="B20">
         <v>50.96335207</v>
@@ -1235,8 +1325,8 @@
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="1">
-        <v>19</v>
+      <c r="A21" s="1" t="s">
+        <v>32</v>
       </c>
       <c r="B21">
         <v>50.96798292</v>
@@ -1276,8 +1366,8 @@
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="1">
-        <v>20</v>
+      <c r="A22" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="B22">
         <v>50.97090515</v>
@@ -1317,8 +1407,8 @@
       </c>
     </row>
     <row r="23" spans="1:13">
-      <c r="A23" s="1">
-        <v>21</v>
+      <c r="A23" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="B23">
         <v>50.96879226</v>
@@ -1358,8 +1448,8 @@
       </c>
     </row>
     <row r="24" spans="1:13">
-      <c r="A24" s="1">
-        <v>22</v>
+      <c r="A24" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B24">
         <v>50.9693878</v>
@@ -1399,8 +1489,8 @@
       </c>
     </row>
     <row r="25" spans="1:13">
-      <c r="A25" s="1">
-        <v>23</v>
+      <c r="A25" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B25">
         <v>50.96613483</v>
@@ -1440,8 +1530,8 @@
       </c>
     </row>
     <row r="26" spans="1:13">
-      <c r="A26" s="1">
-        <v>24</v>
+      <c r="A26" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B26">
         <v>50.96439677</v>
@@ -1481,8 +1571,8 @@
       </c>
     </row>
     <row r="27" spans="1:13">
-      <c r="A27" s="1">
-        <v>25</v>
+      <c r="A27" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B27">
         <v>50.96562536</v>
@@ -1522,8 +1612,8 @@
       </c>
     </row>
     <row r="28" spans="1:13">
-      <c r="A28" s="1">
-        <v>26</v>
+      <c r="A28" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B28">
         <v>50.96513679</v>
@@ -1563,8 +1653,8 @@
       </c>
     </row>
     <row r="29" spans="1:13">
-      <c r="A29" s="1">
-        <v>27</v>
+      <c r="A29" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="B29">
         <v>50.96402757</v>
@@ -1650,7 +1740,7 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="B2">
         <v>0.6279533464311036</v>

</xml_diff>